<commit_message>
tweak map & shorten placeholder description
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -41,7 +41,7 @@
     <t>sugar</t>
   </si>
   <si>
-    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat.</t>
+    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex.</t>
   </si>
   <si>
     <t>season</t>
@@ -106,27 +106,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left>
-        <color indexed="8"/>
-      </left>
-      <right>
-        <color indexed="8"/>
-      </right>
-      <top>
-        <color indexed="8"/>
-      </top>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -222,7 +207,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -232,49 +217,43 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="59" fontId="3" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="59" fontId="3" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1339,7 +1318,7 @@
     <col min="4" max="4" width="9.67188" style="1" customWidth="1"/>
     <col min="5" max="5" width="10.3516" style="1" customWidth="1"/>
     <col min="6" max="6" width="7.67188" style="1" customWidth="1"/>
-    <col min="7" max="7" width="69.8203" style="1" customWidth="1"/>
+    <col min="7" max="7" width="69.8516" style="1" customWidth="1"/>
     <col min="8" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1347,114 +1326,114 @@
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" t="s" s="3">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" t="s" s="3">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" t="s" s="3">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="E1" t="s" s="3">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="2">
+      <c r="F1" t="s" s="3">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="2">
+      <c r="G1" t="s" s="4">
         <v>6</v>
       </c>
     </row>
     <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" s="3">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="2">
+      <c r="B2" t="s" s="6">
         <v>7</v>
       </c>
-      <c r="C2" t="s" s="2">
+      <c r="C2" t="s" s="6">
         <v>8</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="7">
         <v>42.1890292</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="7">
         <v>-72.06167840000001</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="7">
         <v>400</v>
       </c>
-      <c r="G2" t="s" s="2">
+      <c r="G2" t="s" s="8">
         <v>9</v>
       </c>
     </row>
     <row r="3" ht="20.05" customHeight="1">
-      <c r="A3" s="3">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" t="s" s="2">
+      <c r="B3" t="s" s="6">
         <v>7</v>
       </c>
-      <c r="C3" t="s" s="2">
+      <c r="C3" t="s" s="6">
         <v>8</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="7">
         <v>42.1890292</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="7">
         <v>-72.06167840000001</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="7">
         <v>400</v>
       </c>
-      <c r="G3" t="s" s="2">
+      <c r="G3" t="s" s="8">
         <v>9</v>
       </c>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" s="3">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" t="s" s="2">
+      <c r="B4" t="s" s="6">
         <v>7</v>
       </c>
-      <c r="C4" t="s" s="2">
+      <c r="C4" t="s" s="6">
         <v>8</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="7">
         <v>42.1890292</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="7">
         <v>-72.06167840000001</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="7">
         <v>400</v>
       </c>
-      <c r="G4" t="s" s="2">
+      <c r="G4" t="s" s="8">
         <v>9</v>
       </c>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="3">
+      <c r="A5" s="9">
         <v>4</v>
       </c>
-      <c r="B5" t="s" s="2">
+      <c r="B5" t="s" s="10">
         <v>7</v>
       </c>
-      <c r="C5" t="s" s="2">
+      <c r="C5" t="s" s="10">
         <v>8</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="11">
         <v>42.1890292</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="11">
         <v>-72.06167840000001</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="11">
         <v>400</v>
       </c>
-      <c r="G5" t="s" s="2">
+      <c r="G5" t="s" s="12">
         <v>9</v>
       </c>
     </row>
@@ -1478,435 +1457,435 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="6.35156" style="4" customWidth="1"/>
-    <col min="2" max="2" width="3.85156" style="4" customWidth="1"/>
-    <col min="3" max="4" width="9.85156" style="4" customWidth="1"/>
-    <col min="5" max="5" width="4.35156" style="4" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="4" customWidth="1"/>
+    <col min="1" max="1" width="6.35156" style="13" customWidth="1"/>
+    <col min="2" max="2" width="3.85156" style="13" customWidth="1"/>
+    <col min="3" max="4" width="9.85156" style="13" customWidth="1"/>
+    <col min="5" max="5" width="4.35156" style="13" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
-      <c r="A1" t="s" s="5">
+      <c r="A1" t="s" s="2">
         <v>10</v>
       </c>
-      <c r="B1" t="s" s="6">
+      <c r="B1" t="s" s="3">
         <v>11</v>
       </c>
-      <c r="C1" t="s" s="6">
+      <c r="C1" t="s" s="3">
         <v>12</v>
       </c>
-      <c r="D1" t="s" s="6">
+      <c r="D1" t="s" s="3">
         <v>13</v>
       </c>
-      <c r="E1" t="s" s="7">
+      <c r="E1" t="s" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" s="8">
+      <c r="A2" s="5">
         <v>2025</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="7">
         <v>1</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="14">
         <v>45696</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="14">
         <v>45724</v>
       </c>
-      <c r="E2" s="11">
+      <c r="E2" s="15">
         <v>2.5</v>
       </c>
     </row>
     <row r="3" ht="20.05" customHeight="1">
-      <c r="A3" s="8">
+      <c r="A3" s="5">
         <v>2025</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="7">
         <v>2</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="14">
         <v>45696</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="14">
         <v>45724</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="15">
         <v>5</v>
       </c>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" s="8">
+      <c r="A4" s="5">
         <v>2025</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="7">
         <v>3</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="14">
         <v>45696</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="14">
         <v>45724</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="15">
         <v>10</v>
       </c>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="8">
+      <c r="A5" s="5">
         <v>2025</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="7">
         <v>4</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="14">
         <v>45696</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="14">
         <v>45724</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="8">
+      <c r="A6" s="5">
         <v>2026</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="7">
         <v>1</v>
       </c>
-      <c r="C6" t="s" s="12">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s" s="12">
-        <v>15</v>
-      </c>
-      <c r="E6" t="s" s="13">
+      <c r="C6" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s" s="8">
         <v>15</v>
       </c>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="8">
+      <c r="A7" s="5">
         <v>2026</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="7">
         <v>2</v>
       </c>
-      <c r="C7" t="s" s="12">
-        <v>15</v>
-      </c>
-      <c r="D7" t="s" s="12">
-        <v>15</v>
-      </c>
-      <c r="E7" t="s" s="13">
+      <c r="C7" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s" s="8">
         <v>15</v>
       </c>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="8">
+      <c r="A8" s="5">
         <v>2026</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="7">
         <v>3</v>
       </c>
-      <c r="C8" t="s" s="12">
-        <v>15</v>
-      </c>
-      <c r="D8" t="s" s="12">
-        <v>15</v>
-      </c>
-      <c r="E8" t="s" s="13">
+      <c r="C8" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s" s="8">
         <v>15</v>
       </c>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="8">
+      <c r="A9" s="5">
         <v>2026</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="7">
         <v>4</v>
       </c>
-      <c r="C9" t="s" s="12">
-        <v>15</v>
-      </c>
-      <c r="D9" t="s" s="12">
-        <v>15</v>
-      </c>
-      <c r="E9" t="s" s="13">
+      <c r="C9" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s" s="8">
         <v>15</v>
       </c>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="8">
+      <c r="A10" s="5">
         <v>2027</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="7">
         <v>1</v>
       </c>
-      <c r="C10" t="s" s="12">
-        <v>15</v>
-      </c>
-      <c r="D10" t="s" s="12">
-        <v>15</v>
-      </c>
-      <c r="E10" t="s" s="13">
+      <c r="C10" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="E10" t="s" s="8">
         <v>15</v>
       </c>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="8">
+      <c r="A11" s="5">
         <v>2027</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="7">
         <v>2</v>
       </c>
-      <c r="C11" t="s" s="12">
-        <v>15</v>
-      </c>
-      <c r="D11" t="s" s="12">
-        <v>15</v>
-      </c>
-      <c r="E11" t="s" s="13">
+      <c r="C11" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="E11" t="s" s="8">
         <v>15</v>
       </c>
     </row>
     <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" s="8">
+      <c r="A12" s="5">
         <v>2027</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="7">
         <v>3</v>
       </c>
-      <c r="C12" t="s" s="12">
-        <v>15</v>
-      </c>
-      <c r="D12" t="s" s="12">
-        <v>15</v>
-      </c>
-      <c r="E12" t="s" s="13">
+      <c r="C12" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="D12" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="E12" t="s" s="8">
         <v>15</v>
       </c>
     </row>
     <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" s="8">
+      <c r="A13" s="5">
         <v>2027</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="7">
         <v>4</v>
       </c>
-      <c r="C13" t="s" s="12">
-        <v>15</v>
-      </c>
-      <c r="D13" t="s" s="12">
-        <v>15</v>
-      </c>
-      <c r="E13" t="s" s="13">
+      <c r="C13" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="D13" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="E13" t="s" s="8">
         <v>15</v>
       </c>
     </row>
     <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" s="8">
+      <c r="A14" s="5">
         <v>2028</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="7">
         <v>1</v>
       </c>
-      <c r="C14" t="s" s="12">
-        <v>15</v>
-      </c>
-      <c r="D14" t="s" s="12">
-        <v>15</v>
-      </c>
-      <c r="E14" t="s" s="13">
+      <c r="C14" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="D14" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="E14" t="s" s="8">
         <v>15</v>
       </c>
     </row>
     <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="8">
+      <c r="A15" s="5">
         <v>2028</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="7">
         <v>2</v>
       </c>
-      <c r="C15" t="s" s="12">
-        <v>15</v>
-      </c>
-      <c r="D15" t="s" s="12">
-        <v>15</v>
-      </c>
-      <c r="E15" t="s" s="13">
+      <c r="C15" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="D15" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="E15" t="s" s="8">
         <v>15</v>
       </c>
     </row>
     <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" s="8">
+      <c r="A16" s="5">
         <v>2028</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B16" s="7">
         <v>3</v>
       </c>
-      <c r="C16" t="s" s="12">
-        <v>15</v>
-      </c>
-      <c r="D16" t="s" s="12">
-        <v>15</v>
-      </c>
-      <c r="E16" t="s" s="13">
+      <c r="C16" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="D16" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="E16" t="s" s="8">
         <v>15</v>
       </c>
     </row>
     <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" s="8">
+      <c r="A17" s="5">
         <v>2028</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17" s="7">
         <v>4</v>
       </c>
-      <c r="C17" t="s" s="12">
-        <v>15</v>
-      </c>
-      <c r="D17" t="s" s="12">
-        <v>15</v>
-      </c>
-      <c r="E17" t="s" s="13">
+      <c r="C17" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="D17" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="E17" t="s" s="8">
         <v>15</v>
       </c>
     </row>
     <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" s="8">
+      <c r="A18" s="5">
         <v>2029</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18" s="7">
         <v>1</v>
       </c>
-      <c r="C18" t="s" s="12">
-        <v>15</v>
-      </c>
-      <c r="D18" t="s" s="12">
-        <v>15</v>
-      </c>
-      <c r="E18" t="s" s="13">
+      <c r="C18" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="D18" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="E18" t="s" s="8">
         <v>15</v>
       </c>
     </row>
     <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" s="8">
+      <c r="A19" s="5">
         <v>2029</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B19" s="7">
         <v>2</v>
       </c>
-      <c r="C19" t="s" s="12">
-        <v>15</v>
-      </c>
-      <c r="D19" t="s" s="12">
-        <v>15</v>
-      </c>
-      <c r="E19" t="s" s="13">
+      <c r="C19" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="D19" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="E19" t="s" s="8">
         <v>15</v>
       </c>
     </row>
     <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="8">
+      <c r="A20" s="5">
         <v>2029</v>
       </c>
-      <c r="B20" s="9">
+      <c r="B20" s="7">
         <v>3</v>
       </c>
-      <c r="C20" t="s" s="12">
-        <v>15</v>
-      </c>
-      <c r="D20" t="s" s="12">
-        <v>15</v>
-      </c>
-      <c r="E20" t="s" s="13">
+      <c r="C20" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="D20" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="E20" t="s" s="8">
         <v>15</v>
       </c>
     </row>
     <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="8">
+      <c r="A21" s="5">
         <v>2029</v>
       </c>
-      <c r="B21" s="9">
+      <c r="B21" s="7">
         <v>4</v>
       </c>
-      <c r="C21" t="s" s="12">
-        <v>15</v>
-      </c>
-      <c r="D21" t="s" s="12">
-        <v>15</v>
-      </c>
-      <c r="E21" t="s" s="13">
+      <c r="C21" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="D21" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="E21" t="s" s="8">
         <v>15</v>
       </c>
     </row>
     <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" s="8">
+      <c r="A22" s="5">
         <v>2030</v>
       </c>
-      <c r="B22" s="9">
+      <c r="B22" s="7">
         <v>1</v>
       </c>
-      <c r="C22" t="s" s="12">
-        <v>15</v>
-      </c>
-      <c r="D22" t="s" s="12">
-        <v>15</v>
-      </c>
-      <c r="E22" t="s" s="13">
+      <c r="C22" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="D22" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="E22" t="s" s="8">
         <v>15</v>
       </c>
     </row>
     <row r="23" ht="20.05" customHeight="1">
-      <c r="A23" s="8">
+      <c r="A23" s="5">
         <v>2030</v>
       </c>
-      <c r="B23" s="9">
+      <c r="B23" s="7">
         <v>2</v>
       </c>
-      <c r="C23" t="s" s="12">
-        <v>15</v>
-      </c>
-      <c r="D23" t="s" s="12">
-        <v>15</v>
-      </c>
-      <c r="E23" t="s" s="13">
+      <c r="C23" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="D23" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="E23" t="s" s="8">
         <v>15</v>
       </c>
     </row>
     <row r="24" ht="20.05" customHeight="1">
-      <c r="A24" s="8">
+      <c r="A24" s="5">
         <v>2030</v>
       </c>
-      <c r="B24" s="9">
+      <c r="B24" s="7">
         <v>3</v>
       </c>
-      <c r="C24" t="s" s="12">
-        <v>15</v>
-      </c>
-      <c r="D24" t="s" s="12">
-        <v>15</v>
-      </c>
-      <c r="E24" t="s" s="13">
+      <c r="C24" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="D24" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="E24" t="s" s="8">
         <v>15</v>
       </c>
     </row>
     <row r="25" ht="20.05" customHeight="1">
-      <c r="A25" s="14">
+      <c r="A25" s="9">
         <v>2030</v>
       </c>
-      <c r="B25" s="15">
+      <c r="B25" s="11">
         <v>4</v>
       </c>
-      <c r="C25" t="s" s="16">
-        <v>15</v>
-      </c>
-      <c r="D25" t="s" s="16">
-        <v>15</v>
-      </c>
-      <c r="E25" t="s" s="17">
+      <c r="C25" t="s" s="10">
+        <v>15</v>
+      </c>
+      <c r="D25" t="s" s="10">
+        <v>15</v>
+      </c>
+      <c r="E25" t="s" s="12">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add season summary page
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -7,12 +7,13 @@
   <sheets>
     <sheet name="trees" sheetId="1" r:id="rId4"/>
     <sheet name="yields" sheetId="2" r:id="rId5"/>
+    <sheet name="weather" sheetId="3" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
   <si>
     <t>id</t>
   </si>
@@ -61,6 +62,15 @@
   <si>
     <t>-</t>
   </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
 </sst>
 </file>
 
@@ -106,7 +116,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -201,13 +211,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <top>
+        <color indexed="8"/>
+      </top>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -254,6 +279,21 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="59" fontId="3" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1896,4 +1936,1319 @@
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:D92"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="6.35156" style="16" customWidth="1"/>
+    <col min="2" max="2" width="10.5" style="16" customWidth="1"/>
+    <col min="3" max="3" width="3.85156" style="16" customWidth="1"/>
+    <col min="4" max="4" width="3.35156" style="16" customWidth="1"/>
+    <col min="5" max="16384" width="16.3516" style="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="20.25" customHeight="1">
+      <c r="A1" t="s" s="17">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s" s="17">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s" s="17">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s" s="17">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" ht="20.25" customHeight="1">
+      <c r="A2" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B2" s="19">
+        <v>45658</v>
+      </c>
+      <c r="C2" s="18">
+        <v>43</v>
+      </c>
+      <c r="D2" s="18">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" ht="20.05" customHeight="1">
+      <c r="A3" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B3" s="19">
+        <v>45659</v>
+      </c>
+      <c r="C3" s="18">
+        <v>38</v>
+      </c>
+      <c r="D3" s="18">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" ht="20.05" customHeight="1">
+      <c r="A4" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B4" s="19">
+        <v>45660</v>
+      </c>
+      <c r="C4" s="18">
+        <v>34</v>
+      </c>
+      <c r="D4" s="18">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" ht="20.05" customHeight="1">
+      <c r="A5" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B5" s="19">
+        <v>45661</v>
+      </c>
+      <c r="C5" s="18">
+        <v>28</v>
+      </c>
+      <c r="D5" s="18">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" ht="20.05" customHeight="1">
+      <c r="A6" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B6" s="19">
+        <v>45662</v>
+      </c>
+      <c r="C6" s="20">
+        <v>30</v>
+      </c>
+      <c r="D6" s="20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" ht="20.05" customHeight="1">
+      <c r="A7" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B7" s="19">
+        <v>45663</v>
+      </c>
+      <c r="C7" s="20">
+        <v>22</v>
+      </c>
+      <c r="D7" s="20">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" ht="20.05" customHeight="1">
+      <c r="A8" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B8" s="19">
+        <v>45664</v>
+      </c>
+      <c r="C8" s="20">
+        <v>24</v>
+      </c>
+      <c r="D8" s="20">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" ht="20.05" customHeight="1">
+      <c r="A9" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B9" s="19">
+        <v>45665</v>
+      </c>
+      <c r="C9" s="20">
+        <v>24</v>
+      </c>
+      <c r="D9" s="20">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" ht="20.05" customHeight="1">
+      <c r="A10" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B10" s="19">
+        <v>45666</v>
+      </c>
+      <c r="C10" s="20">
+        <v>25</v>
+      </c>
+      <c r="D10" s="20">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" ht="20.05" customHeight="1">
+      <c r="A11" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B11" s="19">
+        <v>45667</v>
+      </c>
+      <c r="C11" s="20">
+        <v>39</v>
+      </c>
+      <c r="D11" s="20">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" ht="20.05" customHeight="1">
+      <c r="A12" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B12" s="19">
+        <v>45668</v>
+      </c>
+      <c r="C12" s="20">
+        <v>30</v>
+      </c>
+      <c r="D12" s="20">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" ht="20.05" customHeight="1">
+      <c r="A13" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B13" s="19">
+        <v>45669</v>
+      </c>
+      <c r="C13" s="20">
+        <v>35</v>
+      </c>
+      <c r="D13" s="20">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" ht="20.05" customHeight="1">
+      <c r="A14" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B14" s="19">
+        <v>45670</v>
+      </c>
+      <c r="C14" s="20">
+        <v>36</v>
+      </c>
+      <c r="D14" s="20">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" ht="20.05" customHeight="1">
+      <c r="A15" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B15" s="19">
+        <v>45671</v>
+      </c>
+      <c r="C15" s="20">
+        <v>28</v>
+      </c>
+      <c r="D15" s="20">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" ht="20.05" customHeight="1">
+      <c r="A16" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B16" s="19">
+        <v>45672</v>
+      </c>
+      <c r="C16" s="20">
+        <v>25</v>
+      </c>
+      <c r="D16" s="20">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" ht="20.05" customHeight="1">
+      <c r="A17" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B17" s="19">
+        <v>45673</v>
+      </c>
+      <c r="C17" s="20">
+        <v>27</v>
+      </c>
+      <c r="D17" s="20">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" ht="20.05" customHeight="1">
+      <c r="A18" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B18" s="19">
+        <v>45674</v>
+      </c>
+      <c r="C18" s="20">
+        <v>33</v>
+      </c>
+      <c r="D18" s="20">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" ht="20.05" customHeight="1">
+      <c r="A19" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B19" s="19">
+        <v>45675</v>
+      </c>
+      <c r="C19" s="20">
+        <v>39</v>
+      </c>
+      <c r="D19" s="20">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" ht="20.05" customHeight="1">
+      <c r="A20" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B20" s="19">
+        <v>45676</v>
+      </c>
+      <c r="C20" s="20">
+        <v>40</v>
+      </c>
+      <c r="D20" s="20">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" ht="20.05" customHeight="1">
+      <c r="A21" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B21" s="19">
+        <v>45677</v>
+      </c>
+      <c r="C21" s="20">
+        <v>22</v>
+      </c>
+      <c r="D21" s="20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" ht="20.05" customHeight="1">
+      <c r="A22" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B22" s="19">
+        <v>45678</v>
+      </c>
+      <c r="C22" s="20">
+        <v>14</v>
+      </c>
+      <c r="D22" s="20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" ht="20.05" customHeight="1">
+      <c r="A23" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B23" s="19">
+        <v>45679</v>
+      </c>
+      <c r="C23" s="20">
+        <v>18</v>
+      </c>
+      <c r="D23" s="20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" ht="20.05" customHeight="1">
+      <c r="A24" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B24" s="19">
+        <v>45680</v>
+      </c>
+      <c r="C24" s="20">
+        <v>26</v>
+      </c>
+      <c r="D24" s="20">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" ht="20.05" customHeight="1">
+      <c r="A25" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B25" s="19">
+        <v>45681</v>
+      </c>
+      <c r="C25" s="20">
+        <v>29</v>
+      </c>
+      <c r="D25" s="20">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" ht="20.05" customHeight="1">
+      <c r="A26" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B26" s="19">
+        <v>45682</v>
+      </c>
+      <c r="C26" s="20">
+        <v>26</v>
+      </c>
+      <c r="D26" s="20">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" ht="20.05" customHeight="1">
+      <c r="A27" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B27" s="19">
+        <v>45683</v>
+      </c>
+      <c r="C27" s="20">
+        <v>35</v>
+      </c>
+      <c r="D27" s="20">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" ht="20.05" customHeight="1">
+      <c r="A28" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B28" s="19">
+        <v>45684</v>
+      </c>
+      <c r="C28" s="20">
+        <v>35</v>
+      </c>
+      <c r="D28" s="20">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" ht="20.05" customHeight="1">
+      <c r="A29" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B29" s="19">
+        <v>45685</v>
+      </c>
+      <c r="C29" s="20">
+        <v>33</v>
+      </c>
+      <c r="D29" s="20">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" ht="20.05" customHeight="1">
+      <c r="A30" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B30" s="19">
+        <v>45686</v>
+      </c>
+      <c r="C30" s="20">
+        <v>42</v>
+      </c>
+      <c r="D30" s="20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" ht="20.05" customHeight="1">
+      <c r="A31" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B31" s="19">
+        <v>45687</v>
+      </c>
+      <c r="C31" s="20">
+        <v>24</v>
+      </c>
+      <c r="D31" s="20">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" ht="20.05" customHeight="1">
+      <c r="A32" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B32" s="19">
+        <v>45688</v>
+      </c>
+      <c r="C32" s="20">
+        <v>40</v>
+      </c>
+      <c r="D32" s="20">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" ht="20.05" customHeight="1">
+      <c r="A33" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B33" s="19">
+        <v>45689</v>
+      </c>
+      <c r="C33" s="20">
+        <v>32</v>
+      </c>
+      <c r="D33" s="20">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" ht="20.05" customHeight="1">
+      <c r="A34" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B34" s="19">
+        <v>45690</v>
+      </c>
+      <c r="C34" s="20">
+        <v>24</v>
+      </c>
+      <c r="D34" s="20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" ht="20.05" customHeight="1">
+      <c r="A35" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B35" s="19">
+        <v>45691</v>
+      </c>
+      <c r="C35" s="20">
+        <v>41</v>
+      </c>
+      <c r="D35" s="20">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" ht="20.05" customHeight="1">
+      <c r="A36" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B36" s="19">
+        <v>45692</v>
+      </c>
+      <c r="C36" s="20">
+        <v>41</v>
+      </c>
+      <c r="D36" s="20">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" ht="20.05" customHeight="1">
+      <c r="A37" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B37" s="19">
+        <v>45693</v>
+      </c>
+      <c r="C37" s="20">
+        <v>26</v>
+      </c>
+      <c r="D37" s="20">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" ht="20.05" customHeight="1">
+      <c r="A38" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B38" s="19">
+        <v>45694</v>
+      </c>
+      <c r="C38" s="20">
+        <v>33</v>
+      </c>
+      <c r="D38" s="20">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" ht="20.05" customHeight="1">
+      <c r="A39" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B39" s="19">
+        <v>45695</v>
+      </c>
+      <c r="C39" s="20">
+        <v>36</v>
+      </c>
+      <c r="D39" s="20">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" ht="20.05" customHeight="1">
+      <c r="A40" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B40" s="19">
+        <v>45696</v>
+      </c>
+      <c r="C40" s="20">
+        <v>30</v>
+      </c>
+      <c r="D40" s="20">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" ht="20.05" customHeight="1">
+      <c r="A41" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B41" s="19">
+        <v>45697</v>
+      </c>
+      <c r="C41" s="20">
+        <v>30</v>
+      </c>
+      <c r="D41" s="20">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" ht="20.05" customHeight="1">
+      <c r="A42" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B42" s="19">
+        <v>45698</v>
+      </c>
+      <c r="C42" s="20">
+        <v>31</v>
+      </c>
+      <c r="D42" s="20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="43" ht="20.05" customHeight="1">
+      <c r="A43" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B43" s="19">
+        <v>45699</v>
+      </c>
+      <c r="C43" s="20">
+        <v>29</v>
+      </c>
+      <c r="D43" s="20">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" ht="20.05" customHeight="1">
+      <c r="A44" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B44" s="19">
+        <v>45700</v>
+      </c>
+      <c r="C44" s="20">
+        <v>29</v>
+      </c>
+      <c r="D44" s="20">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" ht="20.05" customHeight="1">
+      <c r="A45" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B45" s="19">
+        <v>45701</v>
+      </c>
+      <c r="C45" s="20">
+        <v>37</v>
+      </c>
+      <c r="D45" s="20">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="46" ht="20.05" customHeight="1">
+      <c r="A46" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B46" s="19">
+        <v>45702</v>
+      </c>
+      <c r="C46" s="20">
+        <v>30</v>
+      </c>
+      <c r="D46" s="20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="47" ht="20.05" customHeight="1">
+      <c r="A47" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B47" s="19">
+        <v>45703</v>
+      </c>
+      <c r="C47" s="20">
+        <v>26</v>
+      </c>
+      <c r="D47" s="20">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" ht="20.05" customHeight="1">
+      <c r="A48" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B48" s="19">
+        <v>45704</v>
+      </c>
+      <c r="C48" s="20">
+        <v>33</v>
+      </c>
+      <c r="D48" s="20">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="49" ht="20.05" customHeight="1">
+      <c r="A49" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B49" s="19">
+        <v>45705</v>
+      </c>
+      <c r="C49" s="20">
+        <v>25</v>
+      </c>
+      <c r="D49" s="20">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" ht="20.05" customHeight="1">
+      <c r="A50" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B50" s="19">
+        <v>45706</v>
+      </c>
+      <c r="C50" s="20">
+        <v>20</v>
+      </c>
+      <c r="D50" s="20">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="51" ht="20.05" customHeight="1">
+      <c r="A51" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B51" s="19">
+        <v>45707</v>
+      </c>
+      <c r="C51" s="20">
+        <v>26</v>
+      </c>
+      <c r="D51" s="20">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" ht="20.05" customHeight="1">
+      <c r="A52" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B52" s="19">
+        <v>45708</v>
+      </c>
+      <c r="C52" s="20">
+        <v>28</v>
+      </c>
+      <c r="D52" s="20">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" ht="20.05" customHeight="1">
+      <c r="A53" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B53" s="19">
+        <v>45709</v>
+      </c>
+      <c r="C53" s="20">
+        <v>31</v>
+      </c>
+      <c r="D53" s="20">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" ht="20.05" customHeight="1">
+      <c r="A54" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B54" s="19">
+        <v>45710</v>
+      </c>
+      <c r="C54" s="20">
+        <v>32</v>
+      </c>
+      <c r="D54" s="20">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" ht="20.05" customHeight="1">
+      <c r="A55" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B55" s="19">
+        <v>45711</v>
+      </c>
+      <c r="C55" s="20">
+        <v>38</v>
+      </c>
+      <c r="D55" s="20">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" ht="20.05" customHeight="1">
+      <c r="A56" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B56" s="19">
+        <v>45712</v>
+      </c>
+      <c r="C56" s="20">
+        <v>41</v>
+      </c>
+      <c r="D56" s="20">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="57" ht="20.05" customHeight="1">
+      <c r="A57" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B57" s="19">
+        <v>45713</v>
+      </c>
+      <c r="C57" t="s" s="17">
+        <v>15</v>
+      </c>
+      <c r="D57" t="s" s="17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="58" ht="20.05" customHeight="1">
+      <c r="A58" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B58" s="19">
+        <v>45714</v>
+      </c>
+      <c r="C58" t="s" s="17">
+        <v>15</v>
+      </c>
+      <c r="D58" t="s" s="17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="59" ht="20.05" customHeight="1">
+      <c r="A59" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B59" s="19">
+        <v>45715</v>
+      </c>
+      <c r="C59" t="s" s="17">
+        <v>15</v>
+      </c>
+      <c r="D59" t="s" s="17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="60" ht="20.05" customHeight="1">
+      <c r="A60" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B60" s="19">
+        <v>45716</v>
+      </c>
+      <c r="C60" t="s" s="17">
+        <v>15</v>
+      </c>
+      <c r="D60" t="s" s="17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="61" ht="20.05" customHeight="1">
+      <c r="A61" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B61" s="19">
+        <v>45717</v>
+      </c>
+      <c r="C61" t="s" s="17">
+        <v>15</v>
+      </c>
+      <c r="D61" t="s" s="17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="62" ht="20.05" customHeight="1">
+      <c r="A62" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B62" s="19">
+        <v>45718</v>
+      </c>
+      <c r="C62" t="s" s="17">
+        <v>15</v>
+      </c>
+      <c r="D62" t="s" s="17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="63" ht="20.05" customHeight="1">
+      <c r="A63" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B63" s="19">
+        <v>45719</v>
+      </c>
+      <c r="C63" t="s" s="17">
+        <v>15</v>
+      </c>
+      <c r="D63" t="s" s="17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="64" ht="20.05" customHeight="1">
+      <c r="A64" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B64" s="19">
+        <v>45720</v>
+      </c>
+      <c r="C64" t="s" s="17">
+        <v>15</v>
+      </c>
+      <c r="D64" t="s" s="17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="65" ht="20.05" customHeight="1">
+      <c r="A65" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B65" s="19">
+        <v>45721</v>
+      </c>
+      <c r="C65" t="s" s="17">
+        <v>15</v>
+      </c>
+      <c r="D65" t="s" s="17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="66" ht="20.05" customHeight="1">
+      <c r="A66" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B66" s="19">
+        <v>45722</v>
+      </c>
+      <c r="C66" t="s" s="17">
+        <v>15</v>
+      </c>
+      <c r="D66" t="s" s="17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="67" ht="20.05" customHeight="1">
+      <c r="A67" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B67" s="19">
+        <v>45723</v>
+      </c>
+      <c r="C67" t="s" s="17">
+        <v>15</v>
+      </c>
+      <c r="D67" t="s" s="17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="68" ht="20.05" customHeight="1">
+      <c r="A68" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B68" s="19">
+        <v>45724</v>
+      </c>
+      <c r="C68" t="s" s="17">
+        <v>15</v>
+      </c>
+      <c r="D68" t="s" s="17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="69" ht="20.05" customHeight="1">
+      <c r="A69" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B69" s="19">
+        <v>45725</v>
+      </c>
+      <c r="C69" t="s" s="17">
+        <v>15</v>
+      </c>
+      <c r="D69" t="s" s="17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="70" ht="20.05" customHeight="1">
+      <c r="A70" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B70" s="19">
+        <v>45726</v>
+      </c>
+      <c r="C70" t="s" s="17">
+        <v>15</v>
+      </c>
+      <c r="D70" t="s" s="17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="71" ht="20.05" customHeight="1">
+      <c r="A71" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B71" s="19">
+        <v>45727</v>
+      </c>
+      <c r="C71" t="s" s="17">
+        <v>15</v>
+      </c>
+      <c r="D71" t="s" s="17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="72" ht="20.05" customHeight="1">
+      <c r="A72" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B72" s="19">
+        <v>45728</v>
+      </c>
+      <c r="C72" t="s" s="17">
+        <v>15</v>
+      </c>
+      <c r="D72" t="s" s="17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="73" ht="20.05" customHeight="1">
+      <c r="A73" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B73" s="19">
+        <v>45729</v>
+      </c>
+      <c r="C73" t="s" s="17">
+        <v>15</v>
+      </c>
+      <c r="D73" t="s" s="17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="74" ht="20.05" customHeight="1">
+      <c r="A74" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B74" s="19">
+        <v>45730</v>
+      </c>
+      <c r="C74" t="s" s="17">
+        <v>15</v>
+      </c>
+      <c r="D74" t="s" s="17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="75" ht="20.05" customHeight="1">
+      <c r="A75" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B75" s="19">
+        <v>45731</v>
+      </c>
+      <c r="C75" t="s" s="17">
+        <v>15</v>
+      </c>
+      <c r="D75" t="s" s="17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="76" ht="20.05" customHeight="1">
+      <c r="A76" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B76" s="19">
+        <v>45732</v>
+      </c>
+      <c r="C76" t="s" s="17">
+        <v>15</v>
+      </c>
+      <c r="D76" t="s" s="17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="77" ht="20.05" customHeight="1">
+      <c r="A77" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B77" s="19">
+        <v>45733</v>
+      </c>
+      <c r="C77" t="s" s="17">
+        <v>15</v>
+      </c>
+      <c r="D77" t="s" s="17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="78" ht="20.05" customHeight="1">
+      <c r="A78" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B78" s="19">
+        <v>45734</v>
+      </c>
+      <c r="C78" t="s" s="17">
+        <v>15</v>
+      </c>
+      <c r="D78" t="s" s="17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="79" ht="20.05" customHeight="1">
+      <c r="A79" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B79" s="19">
+        <v>45735</v>
+      </c>
+      <c r="C79" t="s" s="17">
+        <v>15</v>
+      </c>
+      <c r="D79" t="s" s="17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="80" ht="20.05" customHeight="1">
+      <c r="A80" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B80" s="19">
+        <v>45736</v>
+      </c>
+      <c r="C80" t="s" s="17">
+        <v>15</v>
+      </c>
+      <c r="D80" t="s" s="17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="81" ht="20.05" customHeight="1">
+      <c r="A81" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B81" s="19">
+        <v>45737</v>
+      </c>
+      <c r="C81" t="s" s="17">
+        <v>15</v>
+      </c>
+      <c r="D81" t="s" s="17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="82" ht="20.05" customHeight="1">
+      <c r="A82" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B82" s="19">
+        <v>45738</v>
+      </c>
+      <c r="C82" t="s" s="17">
+        <v>15</v>
+      </c>
+      <c r="D82" t="s" s="17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="83" ht="20.05" customHeight="1">
+      <c r="A83" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B83" s="19">
+        <v>45739</v>
+      </c>
+      <c r="C83" t="s" s="17">
+        <v>15</v>
+      </c>
+      <c r="D83" t="s" s="17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="84" ht="20.05" customHeight="1">
+      <c r="A84" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B84" s="19">
+        <v>45740</v>
+      </c>
+      <c r="C84" t="s" s="17">
+        <v>15</v>
+      </c>
+      <c r="D84" t="s" s="17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="85" ht="20.05" customHeight="1">
+      <c r="A85" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B85" s="19">
+        <v>45741</v>
+      </c>
+      <c r="C85" t="s" s="17">
+        <v>15</v>
+      </c>
+      <c r="D85" t="s" s="17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="86" ht="20.05" customHeight="1">
+      <c r="A86" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B86" s="19">
+        <v>45742</v>
+      </c>
+      <c r="C86" t="s" s="17">
+        <v>15</v>
+      </c>
+      <c r="D86" t="s" s="17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="87" ht="20.05" customHeight="1">
+      <c r="A87" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B87" s="19">
+        <v>45743</v>
+      </c>
+      <c r="C87" t="s" s="17">
+        <v>15</v>
+      </c>
+      <c r="D87" t="s" s="17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="88" ht="20.05" customHeight="1">
+      <c r="A88" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B88" s="19">
+        <v>45744</v>
+      </c>
+      <c r="C88" t="s" s="17">
+        <v>15</v>
+      </c>
+      <c r="D88" t="s" s="17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="89" ht="20.05" customHeight="1">
+      <c r="A89" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B89" s="19">
+        <v>45745</v>
+      </c>
+      <c r="C89" t="s" s="17">
+        <v>15</v>
+      </c>
+      <c r="D89" t="s" s="17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="90" ht="20.05" customHeight="1">
+      <c r="A90" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B90" s="19">
+        <v>45746</v>
+      </c>
+      <c r="C90" t="s" s="17">
+        <v>15</v>
+      </c>
+      <c r="D90" t="s" s="17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="91" ht="20.05" customHeight="1">
+      <c r="A91" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B91" s="19">
+        <v>45747</v>
+      </c>
+      <c r="C91" t="s" s="17">
+        <v>15</v>
+      </c>
+      <c r="D91" t="s" s="17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="92" ht="20.05" customHeight="1">
+      <c r="A92" s="18">
+        <v>2025</v>
+      </c>
+      <c r="B92" s="19">
+        <v>45748</v>
+      </c>
+      <c r="C92" t="s" s="17">
+        <v>15</v>
+      </c>
+      <c r="D92" t="s" s="17">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>